<commit_message>
Q2 2023 Fiscal Data update
</commit_message>
<xml_diff>
--- a/Data/Fiscal Data/ngdebt.xlsx
+++ b/Data/Fiscal Data/ngdebt.xlsx
@@ -1,1381 +1,1489 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R-Projects\PH-Econ-Data\Data\Fiscal Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B738A553-E5D0-4870-B69E-1AA166642D61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{DF005910-37E0-4F7A-9E42-B5C736A21960}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="ngdebt" sheetId="1" r:id="rId1"/>
-    <sheet name="annual" sheetId="3" r:id="rId2"/>
-    <sheet name="metadata" sheetId="2" r:id="rId3"/>
+    <sheet name="ngdebt" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="annual" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="metadata" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="494">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="494">
   <si>
     <t>Particulars</t>
   </si>
   <si>
-    <t>January 1986</t>
-  </si>
-  <si>
-    <t>February 1986</t>
-  </si>
-  <si>
-    <t>March 1986</t>
-  </si>
-  <si>
-    <t>April 1986</t>
-  </si>
-  <si>
-    <t>May 1986</t>
-  </si>
-  <si>
-    <t>June 1986</t>
-  </si>
-  <si>
-    <t>July 1986</t>
-  </si>
-  <si>
-    <t>August 1986</t>
-  </si>
-  <si>
-    <t>September 1986</t>
-  </si>
-  <si>
-    <t>October 1986</t>
-  </si>
-  <si>
-    <t>November 1986</t>
-  </si>
-  <si>
-    <t>December 1986</t>
-  </si>
-  <si>
-    <t>January 1987</t>
-  </si>
-  <si>
-    <t>February 1987</t>
-  </si>
-  <si>
-    <t>March 1987</t>
-  </si>
-  <si>
-    <t>April 1987</t>
-  </si>
-  <si>
-    <t>May 1987</t>
-  </si>
-  <si>
-    <t>June 1987</t>
-  </si>
-  <si>
-    <t>July 1987</t>
-  </si>
-  <si>
-    <t>August 1987</t>
-  </si>
-  <si>
-    <t>September 1987</t>
-  </si>
-  <si>
-    <t>October 1987</t>
-  </si>
-  <si>
-    <t>November 1987</t>
-  </si>
-  <si>
-    <t>December 1987</t>
-  </si>
-  <si>
-    <t>January 1988</t>
-  </si>
-  <si>
-    <t>February 1988</t>
-  </si>
-  <si>
-    <t>March 1988</t>
-  </si>
-  <si>
-    <t>April 1988</t>
-  </si>
-  <si>
-    <t>May 1988</t>
-  </si>
-  <si>
-    <t>June 1988</t>
-  </si>
-  <si>
-    <t>July 1988</t>
-  </si>
-  <si>
-    <t>August 1988</t>
-  </si>
-  <si>
-    <t>September 1988</t>
-  </si>
-  <si>
-    <t>October 1988</t>
-  </si>
-  <si>
-    <t>November 1988</t>
-  </si>
-  <si>
-    <t>December 1988</t>
-  </si>
-  <si>
-    <t>January 1989</t>
-  </si>
-  <si>
-    <t>February 1989</t>
-  </si>
-  <si>
-    <t>March 1989</t>
-  </si>
-  <si>
-    <t>April 1989</t>
-  </si>
-  <si>
-    <t>May 1989</t>
-  </si>
-  <si>
-    <t>June 1989</t>
-  </si>
-  <si>
-    <t>July 1989</t>
-  </si>
-  <si>
-    <t>August 1989</t>
-  </si>
-  <si>
-    <t>September 1989</t>
-  </si>
-  <si>
-    <t>October 1989</t>
-  </si>
-  <si>
-    <t>November 1989</t>
-  </si>
-  <si>
-    <t>December 1989</t>
-  </si>
-  <si>
-    <t>January 1990</t>
-  </si>
-  <si>
-    <t>February 1990</t>
-  </si>
-  <si>
-    <t>March 1990</t>
-  </si>
-  <si>
-    <t>April 1990</t>
-  </si>
-  <si>
-    <t>May 1990</t>
-  </si>
-  <si>
-    <t>June 1990</t>
-  </si>
-  <si>
-    <t>July 1990</t>
-  </si>
-  <si>
-    <t>August 1990</t>
-  </si>
-  <si>
-    <t>September 1990</t>
-  </si>
-  <si>
-    <t>October 1990</t>
-  </si>
-  <si>
-    <t>November 1990</t>
-  </si>
-  <si>
-    <t>December 1990</t>
-  </si>
-  <si>
-    <t>January 1991</t>
-  </si>
-  <si>
-    <t>February 1991</t>
-  </si>
-  <si>
-    <t>March 1991</t>
-  </si>
-  <si>
-    <t>April 1991</t>
-  </si>
-  <si>
-    <t>May 1991</t>
-  </si>
-  <si>
-    <t>June 1991</t>
-  </si>
-  <si>
-    <t>July 1991</t>
-  </si>
-  <si>
-    <t>August 1991</t>
-  </si>
-  <si>
-    <t>September 1991</t>
-  </si>
-  <si>
-    <t>October 1991</t>
-  </si>
-  <si>
-    <t>November 1991</t>
-  </si>
-  <si>
-    <t>December 1991</t>
-  </si>
-  <si>
-    <t>January 1992</t>
-  </si>
-  <si>
-    <t>February 1992</t>
-  </si>
-  <si>
-    <t>March 1992</t>
-  </si>
-  <si>
-    <t>April 1992</t>
-  </si>
-  <si>
-    <t>May 1992</t>
-  </si>
-  <si>
-    <t>June 1992</t>
-  </si>
-  <si>
-    <t>July 1992</t>
-  </si>
-  <si>
-    <t>August 1992</t>
-  </si>
-  <si>
-    <t>September 1992</t>
-  </si>
-  <si>
-    <t>October 1992</t>
-  </si>
-  <si>
-    <t>November 1992</t>
-  </si>
-  <si>
-    <t>December 1992</t>
-  </si>
-  <si>
-    <t>January 1993</t>
-  </si>
-  <si>
-    <t>February 1993</t>
-  </si>
-  <si>
-    <t>March 1993</t>
-  </si>
-  <si>
-    <t>April 1993</t>
-  </si>
-  <si>
-    <t>May 1993</t>
-  </si>
-  <si>
-    <t>June 1993</t>
-  </si>
-  <si>
-    <t>July 1993</t>
-  </si>
-  <si>
-    <t>August 1993</t>
-  </si>
-  <si>
-    <t>September 1993</t>
-  </si>
-  <si>
-    <t>October 1993</t>
-  </si>
-  <si>
-    <t>November 1993</t>
-  </si>
-  <si>
-    <t>December 1993</t>
-  </si>
-  <si>
-    <t>January 1994</t>
-  </si>
-  <si>
-    <t>February 1994</t>
-  </si>
-  <si>
-    <t>March 1994</t>
-  </si>
-  <si>
-    <t>April 1994</t>
-  </si>
-  <si>
-    <t>May 1994</t>
-  </si>
-  <si>
-    <t>June 1994</t>
-  </si>
-  <si>
-    <t>July 1994</t>
-  </si>
-  <si>
-    <t>August 1994</t>
-  </si>
-  <si>
-    <t>September 1994</t>
-  </si>
-  <si>
-    <t>October 1994</t>
-  </si>
-  <si>
-    <t>November 1994</t>
-  </si>
-  <si>
-    <t>December 1994</t>
-  </si>
-  <si>
-    <t>January 1995</t>
-  </si>
-  <si>
-    <t>February 1995</t>
-  </si>
-  <si>
-    <t>March 1995</t>
-  </si>
-  <si>
-    <t>April 1995</t>
-  </si>
-  <si>
-    <t>May 1995</t>
-  </si>
-  <si>
-    <t>June 1995</t>
-  </si>
-  <si>
-    <t>July 1995</t>
-  </si>
-  <si>
-    <t>August 1995</t>
-  </si>
-  <si>
-    <t>September 1995</t>
-  </si>
-  <si>
-    <t>October 1995</t>
-  </si>
-  <si>
-    <t>November 1995</t>
-  </si>
-  <si>
-    <t>December 1995</t>
-  </si>
-  <si>
-    <t>January 1996</t>
-  </si>
-  <si>
-    <t>February 1996</t>
-  </si>
-  <si>
-    <t>March 1996</t>
-  </si>
-  <si>
-    <t>April 1996</t>
-  </si>
-  <si>
-    <t>May 1996</t>
-  </si>
-  <si>
-    <t>June 1996</t>
-  </si>
-  <si>
-    <t>July 1996</t>
-  </si>
-  <si>
-    <t>August 1996</t>
-  </si>
-  <si>
-    <t>September 1996</t>
-  </si>
-  <si>
-    <t>October 1996</t>
-  </si>
-  <si>
-    <t>November 1996</t>
-  </si>
-  <si>
-    <t>December 1996</t>
-  </si>
-  <si>
-    <t>January 1997</t>
-  </si>
-  <si>
-    <t>February 1997</t>
-  </si>
-  <si>
-    <t>March 1997</t>
-  </si>
-  <si>
-    <t>April 1997</t>
-  </si>
-  <si>
-    <t>May 1997</t>
-  </si>
-  <si>
-    <t>June 1997</t>
-  </si>
-  <si>
-    <t>July 1997</t>
-  </si>
-  <si>
-    <t>August 1997</t>
-  </si>
-  <si>
-    <t>September 1997</t>
-  </si>
-  <si>
-    <t>October 1997</t>
-  </si>
-  <si>
-    <t>November 1997</t>
-  </si>
-  <si>
-    <t>December 1997</t>
-  </si>
-  <si>
-    <t>January 1998</t>
-  </si>
-  <si>
-    <t>February 1998</t>
-  </si>
-  <si>
-    <t>March 1998</t>
-  </si>
-  <si>
-    <t>April 1998</t>
-  </si>
-  <si>
-    <t>May 1998</t>
-  </si>
-  <si>
-    <t>June 1998</t>
-  </si>
-  <si>
-    <t>July 1998</t>
-  </si>
-  <si>
-    <t>August 1998</t>
-  </si>
-  <si>
-    <t>September 1998</t>
-  </si>
-  <si>
-    <t>October 1998</t>
-  </si>
-  <si>
-    <t>November 1998</t>
-  </si>
-  <si>
-    <t>December 1998</t>
-  </si>
-  <si>
-    <t>January 1999</t>
-  </si>
-  <si>
-    <t>February 1999</t>
-  </si>
-  <si>
-    <t>March 1999</t>
-  </si>
-  <si>
-    <t>April 1999</t>
-  </si>
-  <si>
-    <t>May 1999</t>
-  </si>
-  <si>
-    <t>June 1999</t>
-  </si>
-  <si>
-    <t>July 1999</t>
-  </si>
-  <si>
-    <t>August 1999</t>
-  </si>
-  <si>
-    <t>September 1999</t>
-  </si>
-  <si>
-    <t>October 1999</t>
-  </si>
-  <si>
-    <t>November 1999</t>
-  </si>
-  <si>
-    <t>December 1999</t>
-  </si>
-  <si>
-    <t>January 2000</t>
-  </si>
-  <si>
-    <t>February 2000</t>
-  </si>
-  <si>
-    <t>March 2000</t>
-  </si>
-  <si>
-    <t>April 2000</t>
-  </si>
-  <si>
-    <t>May 2000</t>
-  </si>
-  <si>
-    <t>June 2000</t>
-  </si>
-  <si>
-    <t>July 2000</t>
-  </si>
-  <si>
-    <t>August 2000</t>
-  </si>
-  <si>
-    <t>September 2000</t>
-  </si>
-  <si>
-    <t>October 2000</t>
-  </si>
-  <si>
-    <t>November 2000</t>
-  </si>
-  <si>
-    <t>December 2000</t>
-  </si>
-  <si>
-    <t>January 2001</t>
-  </si>
-  <si>
-    <t>February 2001</t>
-  </si>
-  <si>
-    <t>March 2001</t>
-  </si>
-  <si>
-    <t>April 2001</t>
-  </si>
-  <si>
-    <t>May 2001</t>
-  </si>
-  <si>
-    <t>June 2001</t>
-  </si>
-  <si>
-    <t>July 2001</t>
-  </si>
-  <si>
-    <t>August 2001</t>
-  </si>
-  <si>
-    <t>September 2001</t>
-  </si>
-  <si>
-    <t>October 2001</t>
-  </si>
-  <si>
-    <t>November 2001</t>
-  </si>
-  <si>
-    <t>December 2001</t>
-  </si>
-  <si>
-    <t>January 2002</t>
-  </si>
-  <si>
-    <t>February 2002</t>
-  </si>
-  <si>
-    <t>March 2002</t>
-  </si>
-  <si>
-    <t>April 2002</t>
-  </si>
-  <si>
-    <t>May 2002</t>
-  </si>
-  <si>
-    <t>June 2002</t>
-  </si>
-  <si>
-    <t>July 2002</t>
-  </si>
-  <si>
-    <t>August 2002</t>
-  </si>
-  <si>
-    <t>September 2002</t>
-  </si>
-  <si>
-    <t>October 2002</t>
-  </si>
-  <si>
-    <t>November 2002</t>
-  </si>
-  <si>
-    <t>December 2002</t>
-  </si>
-  <si>
-    <t>January 2003</t>
-  </si>
-  <si>
-    <t>February 2003</t>
-  </si>
-  <si>
-    <t>March 2003</t>
-  </si>
-  <si>
-    <t>April 2003</t>
-  </si>
-  <si>
-    <t>May 2003</t>
-  </si>
-  <si>
-    <t>June 2003</t>
-  </si>
-  <si>
-    <t>July 2003</t>
-  </si>
-  <si>
-    <t>August 2003</t>
-  </si>
-  <si>
-    <t>September 2003</t>
-  </si>
-  <si>
-    <t>October 2003</t>
-  </si>
-  <si>
-    <t>November 2003</t>
-  </si>
-  <si>
-    <t>December 2003</t>
-  </si>
-  <si>
-    <t>January 2004</t>
-  </si>
-  <si>
-    <t>February 2004</t>
-  </si>
-  <si>
-    <t>March 2004</t>
-  </si>
-  <si>
-    <t>April 2004</t>
-  </si>
-  <si>
-    <t>May 2004</t>
-  </si>
-  <si>
-    <t>June 2004</t>
-  </si>
-  <si>
-    <t>July 2004</t>
-  </si>
-  <si>
-    <t>August 2004</t>
-  </si>
-  <si>
-    <t>September 2004</t>
-  </si>
-  <si>
-    <t>October 2004</t>
-  </si>
-  <si>
-    <t>November 2004</t>
-  </si>
-  <si>
-    <t>December 2004</t>
-  </si>
-  <si>
-    <t>January 2005</t>
-  </si>
-  <si>
-    <t>February 2005</t>
-  </si>
-  <si>
-    <t>March 2005</t>
-  </si>
-  <si>
-    <t>April 2005</t>
-  </si>
-  <si>
-    <t>May 2005</t>
-  </si>
-  <si>
-    <t>June 2005</t>
-  </si>
-  <si>
-    <t>July 2005</t>
-  </si>
-  <si>
-    <t>August 2005</t>
-  </si>
-  <si>
-    <t>September 2005</t>
-  </si>
-  <si>
-    <t>October 2005</t>
-  </si>
-  <si>
-    <t>November 2005</t>
-  </si>
-  <si>
-    <t>December 2005</t>
-  </si>
-  <si>
-    <t>January 2006</t>
-  </si>
-  <si>
-    <t>February 2006</t>
-  </si>
-  <si>
-    <t>March 2006</t>
-  </si>
-  <si>
-    <t>April 2006</t>
-  </si>
-  <si>
-    <t>May 2006</t>
-  </si>
-  <si>
-    <t>June 2006</t>
-  </si>
-  <si>
-    <t>July 2006</t>
-  </si>
-  <si>
-    <t>August 2006</t>
-  </si>
-  <si>
-    <t>September 2006</t>
-  </si>
-  <si>
-    <t>October 2006</t>
-  </si>
-  <si>
-    <t>November 2006</t>
-  </si>
-  <si>
-    <t>December 2006</t>
-  </si>
-  <si>
-    <t>January 2007</t>
-  </si>
-  <si>
-    <t>February 2007</t>
-  </si>
-  <si>
-    <t>March 2007</t>
-  </si>
-  <si>
-    <t>April 2007</t>
-  </si>
-  <si>
-    <t>May 2007</t>
-  </si>
-  <si>
-    <t>June 2007</t>
-  </si>
-  <si>
-    <t>July 2007</t>
-  </si>
-  <si>
-    <t>August 2007</t>
-  </si>
-  <si>
-    <t>September 2007</t>
-  </si>
-  <si>
-    <t>October 2007</t>
-  </si>
-  <si>
-    <t>November 2007</t>
-  </si>
-  <si>
-    <t>December 2007</t>
-  </si>
-  <si>
-    <t>January 2008</t>
-  </si>
-  <si>
-    <t>February 2008</t>
-  </si>
-  <si>
-    <t>March 2008</t>
-  </si>
-  <si>
-    <t>April 2008</t>
-  </si>
-  <si>
-    <t>May 2008</t>
-  </si>
-  <si>
-    <t>June 2008</t>
-  </si>
-  <si>
-    <t>July 2008</t>
-  </si>
-  <si>
-    <t>August 2008</t>
-  </si>
-  <si>
-    <t>September 2008</t>
-  </si>
-  <si>
-    <t>October 2008</t>
-  </si>
-  <si>
-    <t>November 2008</t>
-  </si>
-  <si>
-    <t>December 2008</t>
-  </si>
-  <si>
-    <t>January 2009</t>
-  </si>
-  <si>
-    <t>February 2009</t>
-  </si>
-  <si>
-    <t>March 2009</t>
-  </si>
-  <si>
-    <t>April 2009</t>
-  </si>
-  <si>
-    <t>May 2009</t>
-  </si>
-  <si>
-    <t>June 2009</t>
-  </si>
-  <si>
-    <t>July 2009</t>
-  </si>
-  <si>
-    <t>August 2009</t>
-  </si>
-  <si>
-    <t>September 2009</t>
-  </si>
-  <si>
-    <t>October 2009</t>
-  </si>
-  <si>
-    <t>November 2009</t>
-  </si>
-  <si>
-    <t>December 2009</t>
-  </si>
-  <si>
-    <t>January 2010</t>
-  </si>
-  <si>
-    <t>February 2010</t>
-  </si>
-  <si>
-    <t>March 2010</t>
-  </si>
-  <si>
-    <t>April 2010</t>
-  </si>
-  <si>
-    <t>May 2010</t>
-  </si>
-  <si>
-    <t>June 2010</t>
-  </si>
-  <si>
-    <t>July 2010</t>
-  </si>
-  <si>
-    <t>August 2010</t>
-  </si>
-  <si>
-    <t>September 2010</t>
-  </si>
-  <si>
-    <t>October 2010</t>
-  </si>
-  <si>
-    <t>November 2010</t>
-  </si>
-  <si>
-    <t>December 2010</t>
-  </si>
-  <si>
-    <t>January 2011</t>
-  </si>
-  <si>
-    <t>February 2011</t>
-  </si>
-  <si>
-    <t>March 2011</t>
-  </si>
-  <si>
-    <t>April 2011</t>
-  </si>
-  <si>
-    <t>May 2011</t>
-  </si>
-  <si>
-    <t>June 2011</t>
-  </si>
-  <si>
-    <t>July 2011</t>
-  </si>
-  <si>
-    <t>August 2011</t>
-  </si>
-  <si>
-    <t>September 2011</t>
-  </si>
-  <si>
-    <t>October 2011</t>
-  </si>
-  <si>
-    <t>November 2011</t>
-  </si>
-  <si>
-    <t>December 2011</t>
-  </si>
-  <si>
-    <t>January 2012</t>
-  </si>
-  <si>
-    <t>February 2012</t>
-  </si>
-  <si>
-    <t>March 2012</t>
-  </si>
-  <si>
-    <t>April 2012</t>
-  </si>
-  <si>
-    <t>May 2012</t>
-  </si>
-  <si>
-    <t>June 2012</t>
-  </si>
-  <si>
-    <t>July 2012</t>
-  </si>
-  <si>
-    <t>August 2012</t>
-  </si>
-  <si>
-    <t>September 2012</t>
-  </si>
-  <si>
-    <t>October 2012</t>
-  </si>
-  <si>
-    <t>November 2012</t>
-  </si>
-  <si>
-    <t>December 2012</t>
-  </si>
-  <si>
-    <t>January 2013</t>
-  </si>
-  <si>
-    <t>February 2013</t>
-  </si>
-  <si>
-    <t>March 2013</t>
-  </si>
-  <si>
-    <t>April 2013</t>
-  </si>
-  <si>
-    <t>May 2013</t>
-  </si>
-  <si>
-    <t>June 2013</t>
-  </si>
-  <si>
-    <t>July 2013</t>
-  </si>
-  <si>
-    <t>August 2013</t>
-  </si>
-  <si>
-    <t>September 2013</t>
-  </si>
-  <si>
-    <t>October 2013</t>
-  </si>
-  <si>
-    <t>November 2013</t>
-  </si>
-  <si>
-    <t>December 2013</t>
-  </si>
-  <si>
-    <t>January 2014</t>
-  </si>
-  <si>
-    <t>February 2014</t>
-  </si>
-  <si>
-    <t>March 2014</t>
-  </si>
-  <si>
-    <t>April 2014</t>
-  </si>
-  <si>
-    <t>May 2014</t>
-  </si>
-  <si>
-    <t>June 2014</t>
-  </si>
-  <si>
-    <t>July 2014</t>
-  </si>
-  <si>
-    <t>August 2014</t>
-  </si>
-  <si>
-    <t>September 2014</t>
-  </si>
-  <si>
-    <t>October 2014</t>
-  </si>
-  <si>
-    <t>November 2014</t>
-  </si>
-  <si>
-    <t>December 2014</t>
-  </si>
-  <si>
-    <t>January 2015</t>
-  </si>
-  <si>
-    <t>February 2015</t>
-  </si>
-  <si>
-    <t>March 2015</t>
-  </si>
-  <si>
-    <t>April 2015</t>
-  </si>
-  <si>
-    <t>May 2015</t>
-  </si>
-  <si>
-    <t>June 2015</t>
-  </si>
-  <si>
-    <t>July 2015</t>
-  </si>
-  <si>
-    <t>August 2015</t>
-  </si>
-  <si>
-    <t>September 2015</t>
-  </si>
-  <si>
-    <t>October 2015</t>
-  </si>
-  <si>
-    <t>November 2015</t>
-  </si>
-  <si>
-    <t>December 2015</t>
-  </si>
-  <si>
-    <t>January 2016</t>
-  </si>
-  <si>
-    <t>February 2016</t>
-  </si>
-  <si>
-    <t>March 2016</t>
-  </si>
-  <si>
-    <t>April 2016</t>
-  </si>
-  <si>
-    <t>May 2016</t>
-  </si>
-  <si>
-    <t>June 2016</t>
-  </si>
-  <si>
-    <t>July 2016</t>
-  </si>
-  <si>
-    <t>August 2016</t>
-  </si>
-  <si>
-    <t>September 2016</t>
-  </si>
-  <si>
-    <t>October 2016</t>
-  </si>
-  <si>
-    <t>November 2016</t>
-  </si>
-  <si>
-    <t>December 2016</t>
-  </si>
-  <si>
-    <t>January 2017</t>
-  </si>
-  <si>
-    <t>February 2017</t>
-  </si>
-  <si>
-    <t>March 2017</t>
-  </si>
-  <si>
-    <t>April 2017</t>
-  </si>
-  <si>
-    <t>May 2017</t>
-  </si>
-  <si>
-    <t>June 2017</t>
-  </si>
-  <si>
-    <t>July 2017</t>
-  </si>
-  <si>
-    <t>August 2017</t>
-  </si>
-  <si>
-    <t>September 2017</t>
-  </si>
-  <si>
-    <t>October 2017</t>
-  </si>
-  <si>
-    <t>November 2017</t>
-  </si>
-  <si>
-    <t>December 2017</t>
-  </si>
-  <si>
-    <t>January 2018</t>
-  </si>
-  <si>
-    <t>February 2018</t>
-  </si>
-  <si>
-    <t>March 2018</t>
-  </si>
-  <si>
-    <t>April 2018</t>
-  </si>
-  <si>
-    <t>May 2018</t>
-  </si>
-  <si>
-    <t>June 2018</t>
-  </si>
-  <si>
-    <t>July 2018</t>
-  </si>
-  <si>
-    <t>August 2018</t>
-  </si>
-  <si>
-    <t>September 2018</t>
-  </si>
-  <si>
-    <t>October 2018</t>
-  </si>
-  <si>
-    <t>November 2018</t>
-  </si>
-  <si>
-    <t>December 2018</t>
-  </si>
-  <si>
-    <t>January 2019</t>
-  </si>
-  <si>
-    <t>February 2019</t>
-  </si>
-  <si>
-    <t>March 2019</t>
-  </si>
-  <si>
-    <t>April 2019</t>
-  </si>
-  <si>
-    <t>May 2019</t>
-  </si>
-  <si>
-    <t>June 2019</t>
-  </si>
-  <si>
-    <t>July 2019</t>
-  </si>
-  <si>
-    <t>August 2019</t>
-  </si>
-  <si>
-    <t>September 2019</t>
-  </si>
-  <si>
-    <t>October 2019</t>
-  </si>
-  <si>
-    <t>November 2019</t>
-  </si>
-  <si>
-    <t>December 2019</t>
-  </si>
-  <si>
-    <t>January 2020</t>
-  </si>
-  <si>
-    <t>February 2020</t>
-  </si>
-  <si>
-    <t>March 2020</t>
-  </si>
-  <si>
-    <t>April 2020</t>
-  </si>
-  <si>
-    <t>May 2020</t>
-  </si>
-  <si>
-    <t>June 2020</t>
-  </si>
-  <si>
-    <t>July 2020</t>
-  </si>
-  <si>
-    <t>August 2020</t>
-  </si>
-  <si>
-    <t>September 2020</t>
-  </si>
-  <si>
-    <t>October 2020</t>
-  </si>
-  <si>
-    <t>November 2020</t>
-  </si>
-  <si>
-    <t>December 2020</t>
-  </si>
-  <si>
-    <t>Actual Obligations</t>
-  </si>
-  <si>
-    <t>Domestic Debt</t>
-  </si>
-  <si>
-    <t>Domestic Debt: Loans</t>
-  </si>
-  <si>
-    <t>Domestic Debt: Debt Securities</t>
-  </si>
-  <si>
-    <t>External Debt</t>
-  </si>
-  <si>
-    <t>External Debt: Loans</t>
-  </si>
-  <si>
-    <t>External Debt: Debt Securities</t>
-  </si>
-  <si>
-    <t>Total Obligations</t>
-  </si>
-  <si>
-    <t>Domestic Guaranteed Obligations</t>
-  </si>
-  <si>
-    <t>External Guaranteed Obligations</t>
-  </si>
-  <si>
-    <t>Guaranteed Obligations</t>
+    <t xml:space="preserve">January 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1986</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1988</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1989</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1990</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1991</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1992</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1994</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1995</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1996</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1997</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1998</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 1999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2013</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">January 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">February 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">March 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">April 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">June 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">August 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">September 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">October 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">November 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">December 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Obligations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Obligations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic Debt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic Debt: Loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic Debt: Debt Securities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Debt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Debt: Loans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Debt: Debt Securities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Guaranteed Obligations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Domestic Guaranteed Obligations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">External Guaranteed Obligations</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t xml:space="preserve">National Government Outstanding Debt</t>
+  </si>
+  <si>
     <t>Source</t>
   </si>
   <si>
-    <t>Bureau of Treasury</t>
+    <t xml:space="preserve">Bureau of Treasury</t>
   </si>
   <si>
     <t>URL</t>
   </si>
   <si>
+    <t>https://www.treasury.gov.ph/?page_id=12407</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other links</t>
+  </si>
+  <si>
+    <t>https://www.foi.gov.ph/requests/aglzfmVmb2ktcGhyHQsSB0NvbnRlbnQiEEJUci05Nzg2NjQyMTk5NjcM</t>
+  </si>
+  <si>
+    <t>https://www.foi.gov.ph/requests/aglzfmVmb2ktcGhyHQsSB0NvbnRlbnQiEEJUci00NjkxMDUxNDgxMjIM</t>
+  </si>
+  <si>
+    <t>https://www.foi.gov.ph/requests/aglzfmVmb2ktcGhyHQsSB0NvbnRlbnQiEEJUci0wNTk2NDY1MjcwNTMM</t>
+  </si>
+  <si>
     <t>Units</t>
   </si>
   <si>
-    <t>Million Pesos</t>
-  </si>
-  <si>
-    <t>Latest Data</t>
+    <t xml:space="preserve">Million Pesos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Latest Data</t>
   </si>
   <si>
     <t>Availability</t>
   </si>
   <si>
-    <t>National Government Outstanding Debt</t>
-  </si>
-  <si>
-    <t>https://www.treasury.gov.ph/?page_id=12407</t>
-  </si>
-  <si>
-    <t>Total (Actual + Guaranteed)</t>
+    <t xml:space="preserve">Total (Actual + Guaranteed)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2009 - 2022</t>
   </si>
   <si>
     <t xml:space="preserve">  Actual Obligations</t>
   </si>
   <si>
+    <t xml:space="preserve">1993 - 2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">    Domestic Debt</t>
   </si>
   <si>
     <t xml:space="preserve">      Loans</t>
   </si>
   <si>
+    <t xml:space="preserve">1995 - 2008; 2009 - 2022</t>
+  </si>
+  <si>
     <t xml:space="preserve">      Debt Securities</t>
   </si>
   <si>
@@ -1389,178 +1497,44 @@
   </si>
   <si>
     <t xml:space="preserve">    External</t>
-  </si>
-  <si>
-    <t>Other links</t>
-  </si>
-  <si>
-    <t>https://www.foi.gov.ph/requests/aglzfmVmb2ktcGhyHQsSB0NvbnRlbnQiEEJUci05Nzg2NjQyMTk5NjcM</t>
-  </si>
-  <si>
-    <t>https://www.foi.gov.ph/requests/aglzfmVmb2ktcGhyHQsSB0NvbnRlbnQiEEJUci00NjkxMDUxNDgxMjIM</t>
-  </si>
-  <si>
-    <t>https://www.foi.gov.ph/requests/aglzfmVmb2ktcGhyHQsSB0NvbnRlbnQiEEJUci0wNTk2NDY1MjcwNTMM</t>
-  </si>
-  <si>
-    <t>January 2021</t>
-  </si>
-  <si>
-    <t>February 2021</t>
-  </si>
-  <si>
-    <t>March 2021</t>
-  </si>
-  <si>
-    <t>April 2021</t>
-  </si>
-  <si>
-    <t>May 2021</t>
-  </si>
-  <si>
-    <t>June 2021</t>
-  </si>
-  <si>
-    <t>July 2021</t>
-  </si>
-  <si>
-    <t>August 2021</t>
-  </si>
-  <si>
-    <t>September 2021</t>
-  </si>
-  <si>
-    <t>October 2021</t>
-  </si>
-  <si>
-    <t>November 2021</t>
-  </si>
-  <si>
-    <t>December 2021</t>
-  </si>
-  <si>
-    <t>January 2022</t>
-  </si>
-  <si>
-    <t>February 2022</t>
-  </si>
-  <si>
-    <t>March 2022</t>
-  </si>
-  <si>
-    <t>April 2022</t>
-  </si>
-  <si>
-    <t>May 2022</t>
-  </si>
-  <si>
-    <t>June 2022</t>
-  </si>
-  <si>
-    <t>July 2022</t>
-  </si>
-  <si>
-    <t>August 2022</t>
-  </si>
-  <si>
-    <t>September 2022</t>
-  </si>
-  <si>
-    <t>October 2022</t>
-  </si>
-  <si>
-    <t>November 2022</t>
-  </si>
-  <si>
-    <t>December 2022</t>
-  </si>
-  <si>
-    <t>2009 - 2022</t>
-  </si>
-  <si>
-    <t>1993 - 2022</t>
-  </si>
-  <si>
-    <t>1995 - 2008; 2009 - 2022</t>
-  </si>
-  <si>
-    <t>January 2023</t>
-  </si>
-  <si>
-    <t>February 2023</t>
-  </si>
-  <si>
-    <t>March 2023</t>
-  </si>
-  <si>
-    <t>April 2023</t>
-  </si>
-  <si>
-    <t>May 2023</t>
-  </si>
-  <si>
-    <t>June 2023</t>
-  </si>
-  <si>
-    <t>July 2023</t>
-  </si>
-  <si>
-    <t>August 2023</t>
-  </si>
-  <si>
-    <t>September 2023</t>
-  </si>
-  <si>
-    <t>October 2023</t>
-  </si>
-  <si>
-    <t>November 2023</t>
-  </si>
-  <si>
-    <t>December 2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
+      <sz val="11.000000"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1573,33 +1547,34 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="8">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="1" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1"/>
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{339237D7-D151-47ED-BD50-CC1BA3D75236}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1607,15 +1582,295 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1657,108 +1912,14 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri Light"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1766,7 +1927,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1792,7 +1953,7 @@
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1844,16 +2005,28 @@
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1869,7 +2042,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1900,33 +2073,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83A7B3-B32D-4D6D-A830-2CD2CA0CA03D}">
-  <dimension ref="A1:QO19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="PZ2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="QG2" sqref="QG2"/>
+    <sheetView zoomScale="80" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="QG2" activeCellId="0" sqref="QG2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="457" width="10.7109375" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="18.28515625"/>
+    <col customWidth="1" min="2" max="457" width="10.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3191,117 +3355,117 @@
         <v>420</v>
       </c>
       <c r="PF1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="PG1" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="PH1" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="PI1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="PJ1" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="PK1" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="PL1" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="PM1" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="PN1" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="PO1" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="PP1" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="PQ1" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="PR1" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="PS1" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="PT1" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="PU1" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="PV1" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="PW1" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="PX1" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="PY1" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="PZ1" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="QA1" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="QB1" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="QC1" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="QD1" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="QE1" s="1" t="s">
+        <v>446</v>
+      </c>
+      <c r="QF1" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="QG1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="QH1" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="QI1" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="QJ1" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="QK1" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="QL1" s="1" t="s">
+        <v>453</v>
+      </c>
+      <c r="QM1" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="QN1" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="PG1" s="1" t="s">
+      <c r="QO1" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="PH1" s="1" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>457</v>
-      </c>
-      <c r="PI1" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="PJ1" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="PK1" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="PL1" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="PM1" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="PN1" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="PO1" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="PP1" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="PQ1" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="PR1" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="PS1" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="PT1" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="PU1" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="PV1" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="PW1" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="PX1" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="PY1" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="PZ1" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="QA1" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="QB1" s="1" t="s">
-        <v>477</v>
-      </c>
-      <c r="QC1" s="1" t="s">
-        <v>478</v>
-      </c>
-      <c r="QD1" s="1" t="s">
-        <v>482</v>
-      </c>
-      <c r="QE1" s="1" t="s">
-        <v>483</v>
-      </c>
-      <c r="QF1" s="1" t="s">
-        <v>484</v>
-      </c>
-      <c r="QG1" s="1" t="s">
-        <v>485</v>
-      </c>
-      <c r="QH1" s="1" t="s">
-        <v>486</v>
-      </c>
-      <c r="QI1" s="1" t="s">
-        <v>487</v>
-      </c>
-      <c r="QJ1" s="1" t="s">
-        <v>488</v>
-      </c>
-      <c r="QK1" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="QL1" s="1" t="s">
-        <v>490</v>
-      </c>
-      <c r="QM1" s="1" t="s">
-        <v>491</v>
-      </c>
-      <c r="QN1" s="1" t="s">
-        <v>492</v>
-      </c>
-      <c r="QO1" s="1" t="s">
-        <v>493</v>
-      </c>
-    </row>
-    <row r="2" spans="1:457" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>428</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -4092,9 +4256,15 @@
       <c r="QF2" s="2">
         <v>14241014</v>
       </c>
-      <c r="QG2" s="2"/>
-      <c r="QH2" s="2"/>
-      <c r="QI2" s="2"/>
+      <c r="QG2" s="2">
+        <v>14291833</v>
+      </c>
+      <c r="QH2" s="2">
+        <v>14476254</v>
+      </c>
+      <c r="QI2" s="2">
+        <v>14517577</v>
+      </c>
       <c r="QJ2" s="2"/>
       <c r="QK2" s="2"/>
       <c r="QL2" s="2"/>
@@ -4102,9 +4272,9 @@
       <c r="QN2" s="2"/>
       <c r="QO2" s="2"/>
     </row>
-    <row r="3" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -4401,7 +4571,7 @@
         <v>1487974.9482499999</v>
       </c>
       <c r="EZ3" s="2">
-        <v>1461038.64</v>
+        <v>1461038.6399999999</v>
       </c>
       <c r="FA3" s="2">
         <v>1496221.764</v>
@@ -4647,7 +4817,7 @@
         <v>3941774.017</v>
       </c>
       <c r="ID3" s="2">
-        <v>4018868.36</v>
+        <v>4018868.3599999999</v>
       </c>
       <c r="IE3" s="2">
         <v>3951689</v>
@@ -5279,9 +5449,15 @@
       <c r="QF3" s="2">
         <v>13856896</v>
       </c>
-      <c r="QG3" s="2"/>
-      <c r="QH3" s="2"/>
-      <c r="QI3" s="2"/>
+      <c r="QG3" s="2">
+        <v>13911139</v>
+      </c>
+      <c r="QH3" s="2">
+        <v>14096542</v>
+      </c>
+      <c r="QI3" s="2">
+        <v>14147850</v>
+      </c>
       <c r="QJ3" s="2"/>
       <c r="QK3" s="2"/>
       <c r="QL3" s="2"/>
@@ -5289,9 +5465,9 @@
       <c r="QN3" s="2"/>
       <c r="QO3" s="2"/>
     </row>
-    <row r="4" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>422</v>
+        <v>459</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -5588,7 +5764,7 @@
         <v>822295.13</v>
       </c>
       <c r="EZ4" s="2">
-        <v>832966.46</v>
+        <v>832966.45999999996</v>
       </c>
       <c r="FA4" s="2">
         <v>850931.05999999994</v>
@@ -6466,9 +6642,15 @@
       <c r="QF4" s="2">
         <v>9513160</v>
       </c>
-      <c r="QG4" s="2"/>
-      <c r="QH4" s="2"/>
-      <c r="QI4" s="2"/>
+      <c r="QG4" s="2">
+        <v>9457840</v>
+      </c>
+      <c r="QH4" s="2">
+        <v>9588514</v>
+      </c>
+      <c r="QI4" s="2">
+        <v>9702829</v>
+      </c>
       <c r="QJ4" s="2"/>
       <c r="QK4" s="2"/>
       <c r="QL4" s="2"/>
@@ -6476,9 +6658,9 @@
       <c r="QN4" s="2"/>
       <c r="QO4" s="2"/>
     </row>
-    <row r="5" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
-        <v>423</v>
+        <v>460</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -6724,13 +6906,13 @@
         <v>71132.941999999995</v>
       </c>
       <c r="EY5" s="2">
-        <v>67510.13</v>
+        <v>67510.130000000005</v>
       </c>
       <c r="EZ5" s="2">
         <v>65832.460000000006</v>
       </c>
       <c r="FA5" s="2">
-        <v>63144.06</v>
+        <v>63144.059999999998</v>
       </c>
       <c r="FB5" s="2">
         <v>62738.016000000003</v>
@@ -7605,9 +7787,15 @@
       <c r="QF5" s="2">
         <v>156</v>
       </c>
-      <c r="QG5" s="2"/>
-      <c r="QH5" s="2"/>
-      <c r="QI5" s="2"/>
+      <c r="QG5" s="2">
+        <v>156</v>
+      </c>
+      <c r="QH5" s="2">
+        <v>156</v>
+      </c>
+      <c r="QI5" s="2">
+        <v>156</v>
+      </c>
       <c r="QJ5" s="2"/>
       <c r="QK5" s="2"/>
       <c r="QL5" s="2"/>
@@ -7615,9 +7803,9 @@
       <c r="QN5" s="2"/>
       <c r="QO5" s="2"/>
     </row>
-    <row r="6" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
-        <v>424</v>
+        <v>461</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -8744,9 +8932,15 @@
       <c r="QF6" s="2">
         <v>9513004</v>
       </c>
-      <c r="QG6" s="2"/>
-      <c r="QH6" s="2"/>
-      <c r="QI6" s="2"/>
+      <c r="QG6" s="2">
+        <v>9457684</v>
+      </c>
+      <c r="QH6" s="2">
+        <v>9588358</v>
+      </c>
+      <c r="QI6" s="2">
+        <v>9702673</v>
+      </c>
       <c r="QJ6" s="2"/>
       <c r="QK6" s="2"/>
       <c r="QL6" s="2"/>
@@ -8754,9 +8948,9 @@
       <c r="QN6" s="2"/>
       <c r="QO6" s="2"/>
     </row>
-    <row r="7" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
-        <v>425</v>
+        <v>462</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -9931,9 +10125,15 @@
       <c r="QF7" s="2">
         <v>4343736</v>
       </c>
-      <c r="QG7" s="2"/>
-      <c r="QH7" s="2"/>
-      <c r="QI7" s="2"/>
+      <c r="QG7" s="2">
+        <v>4453299</v>
+      </c>
+      <c r="QH7" s="2">
+        <v>4508028</v>
+      </c>
+      <c r="QI7" s="2">
+        <v>4445021</v>
+      </c>
       <c r="QJ7" s="2"/>
       <c r="QK7" s="2"/>
       <c r="QL7" s="2"/>
@@ -9941,9 +10141,9 @@
       <c r="QN7" s="2"/>
       <c r="QO7" s="2"/>
     </row>
-    <row r="8" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
-        <v>426</v>
+        <v>463</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -10192,7 +10392,7 @@
         <v>513270.97824999999</v>
       </c>
       <c r="EZ8" s="2">
-        <v>481514.29</v>
+        <v>481514.28999999998</v>
       </c>
       <c r="FA8" s="2">
         <v>500479.054</v>
@@ -10438,7 +10638,7 @@
         <v>795042.01699999999</v>
       </c>
       <c r="ID8" s="2">
-        <v>783468.36</v>
+        <v>783468.35999999999</v>
       </c>
       <c r="IE8" s="2">
         <v>744580</v>
@@ -11070,9 +11270,15 @@
       <c r="QF8" s="2">
         <v>1947472</v>
       </c>
-      <c r="QG8" s="2"/>
-      <c r="QH8" s="2"/>
-      <c r="QI8" s="2"/>
+      <c r="QG8" s="2">
+        <v>2006693</v>
+      </c>
+      <c r="QH8" s="2">
+        <v>2036246</v>
+      </c>
+      <c r="QI8" s="2">
+        <v>2009725</v>
+      </c>
       <c r="QJ8" s="2"/>
       <c r="QK8" s="2"/>
       <c r="QL8" s="2"/>
@@ -11080,9 +11286,9 @@
       <c r="QN8" s="2"/>
       <c r="QO8" s="2"/>
     </row>
-    <row r="9" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
-        <v>427</v>
+        <v>464</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -11334,7 +11540,7 @@
         <v>146557.89000000001</v>
       </c>
       <c r="FA9" s="2">
-        <v>144811.65</v>
+        <v>144811.64999999999</v>
       </c>
       <c r="FB9" s="2">
         <v>182023</v>
@@ -12209,9 +12415,15 @@
       <c r="QF9" s="2">
         <v>2396264</v>
       </c>
-      <c r="QG9" s="2"/>
-      <c r="QH9" s="2"/>
-      <c r="QI9" s="2"/>
+      <c r="QG9" s="2">
+        <v>2446606</v>
+      </c>
+      <c r="QH9" s="2">
+        <v>2471782</v>
+      </c>
+      <c r="QI9" s="2">
+        <v>2435296</v>
+      </c>
       <c r="QJ9" s="2"/>
       <c r="QK9" s="2"/>
       <c r="QL9" s="2"/>
@@ -12219,9 +12431,9 @@
       <c r="QN9" s="2"/>
       <c r="QO9" s="2"/>
     </row>
-    <row r="10" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
-        <v>431</v>
+        <v>465</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -12533,7 +12745,7 @@
         <v>569571</v>
       </c>
       <c r="KC10" s="2">
-        <v>614133.29</v>
+        <v>614133.29000000004</v>
       </c>
       <c r="KD10" s="2">
         <v>619741</v>
@@ -13012,9 +13224,15 @@
       <c r="QF10" s="2">
         <v>384118</v>
       </c>
-      <c r="QG10" s="2"/>
-      <c r="QH10" s="2"/>
-      <c r="QI10" s="2"/>
+      <c r="QG10" s="2">
+        <v>380694</v>
+      </c>
+      <c r="QH10" s="2">
+        <v>379712</v>
+      </c>
+      <c r="QI10" s="2">
+        <v>369727</v>
+      </c>
       <c r="QJ10" s="2"/>
       <c r="QK10" s="2"/>
       <c r="QL10" s="2"/>
@@ -13022,9 +13240,9 @@
       <c r="QN10" s="2"/>
       <c r="QO10" s="2"/>
     </row>
-    <row r="11" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
-        <v>429</v>
+        <v>466</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -13815,9 +14033,15 @@
       <c r="QF11" s="2">
         <v>202083</v>
       </c>
-      <c r="QG11" s="2"/>
-      <c r="QH11" s="2"/>
-      <c r="QI11" s="2"/>
+      <c r="QG11" s="2">
+        <v>196575</v>
+      </c>
+      <c r="QH11" s="2">
+        <v>200734</v>
+      </c>
+      <c r="QI11" s="2">
+        <v>196371</v>
+      </c>
       <c r="QJ11" s="2"/>
       <c r="QK11" s="2"/>
       <c r="QL11" s="2"/>
@@ -13825,9 +14049,9 @@
       <c r="QN11" s="2"/>
       <c r="QO11" s="2"/>
     </row>
-    <row r="12" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
-        <v>430</v>
+        <v>467</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -14139,7 +14363,7 @@
         <v>488052</v>
       </c>
       <c r="KC12" s="2">
-        <v>534614.29</v>
+        <v>534614.29000000004</v>
       </c>
       <c r="KD12" s="2">
         <v>540223</v>
@@ -14618,9 +14842,15 @@
       <c r="QF12" s="2">
         <v>182035</v>
       </c>
-      <c r="QG12" s="2"/>
-      <c r="QH12" s="2"/>
-      <c r="QI12" s="2"/>
+      <c r="QG12" s="2">
+        <v>184119</v>
+      </c>
+      <c r="QH12" s="2">
+        <v>178978</v>
+      </c>
+      <c r="QI12" s="2">
+        <v>173356</v>
+      </c>
       <c r="QJ12" s="2"/>
       <c r="QK12" s="2"/>
       <c r="QL12" s="2"/>
@@ -14628,38 +14858,37 @@
       <c r="QN12" s="2"/>
       <c r="QO12" s="2"/>
     </row>
-    <row r="14" spans="1:457" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="PE14" s="2"/>
       <c r="PQ14" s="2"/>
     </row>
-    <row r="19" spans="421:433" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="PE19" s="2"/>
       <c r="PQ19" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C02CD3A-99C8-4C95-BFC1-453A97FD647F}">
-  <dimension ref="A1:AV4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AN2" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AV5" sqref="AV5"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="AV5" activeCellId="0" sqref="AV5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="48" width="10" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="17.140625"/>
+    <col customWidth="1" min="2" max="48" width="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14805,9 +15034,9 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
-        <v>421</v>
+        <v>458</v>
       </c>
       <c r="B2" s="2">
         <v>26887</v>
@@ -14951,9 +15180,9 @@
         <v>13418860</v>
       </c>
     </row>
-    <row r="3" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
-        <v>422</v>
+        <v>459</v>
       </c>
       <c r="B3" s="2">
         <v>15047</v>
@@ -15097,9 +15326,9 @@
         <v>9208387</v>
       </c>
     </row>
-    <row r="4" spans="1:48" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
-        <v>425</v>
+        <v>462</v>
       </c>
       <c r="B4" s="2">
         <v>11840</v>
@@ -15244,178 +15473,179 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5896838-F7D9-4F29-9E42-CDFCD60FC5B6}">
-  <dimension ref="A1:B21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="100" workbookViewId="0">
+      <selection activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="36.5703125" customWidth="1"/>
+    <col customWidth="1" min="1" max="2" width="36.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="3" t="s">
-        <v>432</v>
+        <v>468</v>
       </c>
       <c r="B1" t="s">
-        <v>440</v>
+        <v>469</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="3" t="s">
-        <v>433</v>
+        <v>470</v>
       </c>
       <c r="B2" t="s">
-        <v>434</v>
+        <v>471</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" s="3" t="s">
-        <v>435</v>
+        <v>472</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>441</v>
+        <v>473</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>451</v>
+    <row r="4">
+      <c r="A4" s="5" t="s">
+        <v>474</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>452</v>
+        <v>475</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+    <row r="5">
+      <c r="A5" s="5"/>
       <c r="B5" s="4" t="s">
-        <v>453</v>
+        <v>476</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+    <row r="6">
+      <c r="A6" s="5"/>
       <c r="B6" s="4" t="s">
-        <v>454</v>
+        <v>477</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" s="3" t="s">
-        <v>436</v>
+        <v>478</v>
       </c>
       <c r="B7" t="s">
-        <v>437</v>
+        <v>479</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" s="3" t="s">
-        <v>438</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>478</v>
+        <v>480</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>450</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10">
+      <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>439</v>
+      <c r="B10" s="7" t="s">
+        <v>481</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="3" t="s">
-        <v>442</v>
+        <v>482</v>
       </c>
       <c r="B11" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="3" t="s">
-        <v>443</v>
+        <v>484</v>
       </c>
       <c r="B12" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="3" t="s">
-        <v>444</v>
+        <v>486</v>
       </c>
       <c r="B13" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
-        <v>445</v>
+        <v>487</v>
       </c>
       <c r="B14" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" t="s">
-        <v>446</v>
+        <v>489</v>
       </c>
       <c r="B15" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="3" t="s">
-        <v>447</v>
+        <v>490</v>
       </c>
       <c r="B16" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s">
-        <v>445</v>
+        <v>487</v>
       </c>
       <c r="B17" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
-        <v>446</v>
+        <v>489</v>
       </c>
       <c r="B18" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="3" t="s">
-        <v>448</v>
+        <v>491</v>
       </c>
       <c r="B19" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="3" t="s">
-        <v>449</v>
+        <v>492</v>
       </c>
       <c r="B20" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="3" t="s">
-        <v>450</v>
+        <v>493</v>
       </c>
       <c r="B21" t="s">
-        <v>479</v>
+        <v>483</v>
       </c>
     </row>
   </sheetData>
@@ -15423,10 +15653,12 @@
     <mergeCell ref="A4:A6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{AA9FBDC1-6B6C-4B8A-AAB8-6A4289FCE0B5}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{3416715F-802A-47CE-A894-BCD6E595154C}"/>
+    <hyperlink r:id="rId1" ref="B3"/>
+    <hyperlink r:id="rId2" ref="B4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>